<commit_message>
RDM-1831 Clean up 2 columns in CaseEventToFields tab and add correct description for 2 new columns in CaseTypeTab.
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V29_RDM-1831.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V29_RDM-1831.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-14060" yWindow="-28340" windowWidth="51200" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="-5640" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="273">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -619,9 +619,6 @@
 Integer</t>
   </si>
   <si>
-    <t>Accepted boolean  values(case Insensitive):Yes/No,Y/N,T/F,True/False</t>
-  </si>
-  <si>
     <t>Boolean expression rules for hiding a page: MaxLength:1000</t>
   </si>
   <si>
@@ -649,9 +646,6 @@
     <t>PageFieldDisplayOrder</t>
   </si>
   <si>
-    <t>ReadOnly</t>
-  </si>
-  <si>
     <t>Mandatory</t>
   </si>
   <si>
@@ -667,9 +661,6 @@
     <t>Personal Information</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>AddressPage</t>
   </si>
   <si>
@@ -874,9 +865,6 @@
     <t>Optional</t>
   </si>
   <si>
-    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;</t>
-  </si>
-  <si>
     <t>TabShowCondition</t>
   </si>
   <si>
@@ -884,6 +872,12 @@
   </si>
   <si>
     <t>PersonLastName="Sparrow"</t>
+  </si>
+  <si>
+    <t>Boolean expression rules for hiding a tab field: MaxLength:1000</t>
+  </si>
+  <si>
+    <t>Boolean expression rules for hiding a tab: MaxLength:1000</t>
   </si>
 </sst>
 </file>
@@ -905,19 +899,19 @@
       <b/>
       <sz val="14"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -944,19 +938,19 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1014,34 +1008,34 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1075,7 +1069,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -2176,7 +2170,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2202,7 +2196,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>5</v>
@@ -2227,7 +2221,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>37</v>
@@ -2345,7 +2339,7 @@
         <v>81</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F8" s="47">
         <v>3</v>
@@ -2539,7 +2533,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B1" s="59" t="s">
         <v>1</v>
@@ -2557,13 +2551,13 @@
       <c r="A2" s="63"/>
       <c r="B2" s="63"/>
       <c r="C2" s="64" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D2" s="64" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F2" s="64" t="s">
         <v>156</v>
@@ -2580,7 +2574,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="65" t="s">
         <v>37</v>
@@ -2853,7 +2847,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2879,7 +2873,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>5</v>
@@ -2904,7 +2898,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>37</v>
@@ -3199,8 +3193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3221,7 +3215,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="7" t="s">
@@ -3256,21 +3250,23 @@
         <v>4</v>
       </c>
       <c r="F2" s="66" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G2" s="66" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H2" s="66" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="66" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J2" s="123" t="s">
+        <v>272</v>
+      </c>
+      <c r="K2" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="K2" s="124"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -3286,28 +3282,28 @@
         <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="H3" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="J3" s="125" t="s">
         <v>118</v>
       </c>
       <c r="K3" s="125" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -3322,10 +3318,10 @@
         <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F4" s="53" t="s">
         <v>10</v>
@@ -3341,7 +3337,7 @@
       </c>
       <c r="J4"/>
       <c r="K4" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
@@ -3356,10 +3352,10 @@
         <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F5" s="53" t="s">
         <v>10</v>
@@ -3374,7 +3370,7 @@
         <v>2</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="K5"/>
       <c r="L5" s="4"/>
@@ -3390,10 +3386,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F6" s="53" t="s">
         <v>55</v>
@@ -3422,10 +3418,10 @@
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F7" s="53" t="s">
         <v>10</v>
@@ -3454,10 +3450,10 @@
         <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F8" s="53" t="s">
         <v>10</v>
@@ -3486,10 +3482,10 @@
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F9" s="53" t="s">
         <v>55</v>
@@ -3518,13 +3514,13 @@
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F10" s="53" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G10" s="4">
         <v>3</v>
@@ -3550,13 +3546,13 @@
         <v>27</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G11" s="4">
         <v>3</v>
@@ -3582,13 +3578,13 @@
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F12" s="53" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G12" s="4">
         <v>3</v>
@@ -3614,13 +3610,13 @@
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>79</v>
       </c>
       <c r="F13" s="53" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G13" s="4">
         <v>4</v>
@@ -3646,13 +3642,13 @@
         <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>81</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G14" s="4">
         <v>3</v>
@@ -3678,13 +3674,13 @@
         <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>84</v>
       </c>
       <c r="F15" s="53" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G15" s="4">
         <v>3</v>
@@ -3710,13 +3706,13 @@
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>85</v>
       </c>
       <c r="F16" s="53" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G16" s="4">
         <v>3</v>
@@ -3925,7 +3921,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3965,16 +3961,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>241</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>244</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -3990,7 +3986,7 @@
         <v>42737</v>
       </c>
       <c r="C4" s="70" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D4" s="71" t="s">
         <v>12</v>
@@ -4015,7 +4011,7 @@
         <v>42737</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D5" s="75" t="s">
         <v>12</v>
@@ -4130,7 +4126,7 @@
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -4400,10 +4396,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -4667,10 +4663,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -4932,10 +4928,10 @@
         <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -5197,10 +5193,10 @@
         <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -5462,10 +5458,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -5727,10 +5723,10 @@
         <v>27</v>
       </c>
       <c r="D7" s="71" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -5992,10 +5988,10 @@
         <v>27</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E8" s="82" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -6257,10 +6253,10 @@
         <v>27</v>
       </c>
       <c r="D9" s="78" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" s="32" t="s">
         <v>256</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>259</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -6797,7 +6793,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B1" s="85" t="s">
         <v>1</v>
@@ -6829,7 +6825,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G2" s="88"/>
       <c r="H2" s="88"/>
@@ -6848,13 +6844,13 @@
         <v>36</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="92" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F3" s="92" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G3" s="93"/>
       <c r="H3" s="93"/>
@@ -6874,10 +6870,10 @@
         <v>45</v>
       </c>
       <c r="E4" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F4" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G4" s="95"/>
       <c r="H4" s="95"/>
@@ -6897,10 +6893,10 @@
         <v>45</v>
       </c>
       <c r="E5" s="96" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F5" s="96" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G5" s="95"/>
       <c r="H5" s="95"/>
@@ -6920,10 +6916,10 @@
         <v>45</v>
       </c>
       <c r="E6" s="96" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F6" s="96" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G6" s="95"/>
       <c r="H6" s="95"/>
@@ -6943,10 +6939,10 @@
         <v>52</v>
       </c>
       <c r="E7" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F7" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G7" s="95"/>
       <c r="H7" s="95"/>
@@ -6966,10 +6962,10 @@
         <v>52</v>
       </c>
       <c r="E8" s="96" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F8" s="96" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G8" s="95"/>
       <c r="H8" s="95"/>
@@ -6989,10 +6985,10 @@
         <v>52</v>
       </c>
       <c r="E9" s="96" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F9" s="96" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
@@ -7012,10 +7008,10 @@
         <v>54</v>
       </c>
       <c r="E10" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F10" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
@@ -7035,10 +7031,10 @@
         <v>54</v>
       </c>
       <c r="E11" s="96" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F11" s="96" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
@@ -7058,10 +7054,10 @@
         <v>54</v>
       </c>
       <c r="E12" s="96" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F12" s="96" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G12" s="95"/>
       <c r="H12" s="95"/>
@@ -7081,10 +7077,10 @@
         <v>50</v>
       </c>
       <c r="E13" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F13" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G13" s="95"/>
       <c r="H13" s="95"/>
@@ -7104,10 +7100,10 @@
         <v>45</v>
       </c>
       <c r="E14" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F14" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G14" s="95"/>
       <c r="H14" s="95"/>
@@ -7127,10 +7123,10 @@
         <v>52</v>
       </c>
       <c r="E15" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F15" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G15" s="95"/>
       <c r="H15" s="95"/>
@@ -7150,10 +7146,10 @@
         <v>54</v>
       </c>
       <c r="E16" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F16" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G16" s="95"/>
       <c r="H16" s="95"/>
@@ -7173,10 +7169,10 @@
         <v>71</v>
       </c>
       <c r="E17" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F17" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G17" s="95"/>
       <c r="H17" s="95"/>
@@ -7196,10 +7192,10 @@
         <v>74</v>
       </c>
       <c r="E18" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F18" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G18" s="95"/>
       <c r="H18" s="95"/>
@@ -7219,10 +7215,10 @@
         <v>77</v>
       </c>
       <c r="E19" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F19" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G19" s="95"/>
       <c r="H19" s="95"/>
@@ -7242,10 +7238,10 @@
         <v>79</v>
       </c>
       <c r="E20" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F20" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G20" s="95"/>
       <c r="H20" s="95"/>
@@ -7265,10 +7261,10 @@
         <v>81</v>
       </c>
       <c r="E21" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F21" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G21" s="95"/>
       <c r="H21" s="95"/>
@@ -7288,10 +7284,10 @@
         <v>84</v>
       </c>
       <c r="E22" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F22" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G22" s="95"/>
       <c r="H22" s="95"/>
@@ -7311,10 +7307,10 @@
         <v>85</v>
       </c>
       <c r="E23" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F23" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G23" s="95"/>
       <c r="H23" s="95"/>
@@ -7334,10 +7330,10 @@
         <v>89</v>
       </c>
       <c r="E24" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F24" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G24" s="95"/>
       <c r="H24" s="95"/>
@@ -7357,10 +7353,10 @@
         <v>93</v>
       </c>
       <c r="E25" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F25" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G25" s="95"/>
       <c r="H25" s="95"/>
@@ -7380,10 +7376,10 @@
         <v>96</v>
       </c>
       <c r="E26" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F26" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G26" s="95"/>
       <c r="H26" s="95"/>
@@ -7403,10 +7399,10 @@
         <v>56</v>
       </c>
       <c r="E27" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F27" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G27" s="95"/>
       <c r="H27" s="95"/>
@@ -7426,10 +7422,10 @@
         <v>59</v>
       </c>
       <c r="E28" s="96" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F28" s="96" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G28" s="95"/>
       <c r="H28" s="95"/>
@@ -7763,7 +7759,7 @@
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -8036,10 +8032,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -8302,13 +8298,13 @@
         <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -8572,10 +8568,10 @@
         <v>170</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -8839,10 +8835,10 @@
         <v>170</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -9106,10 +9102,10 @@
         <v>170</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -9373,10 +9369,10 @@
         <v>173</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -9640,10 +9636,10 @@
         <v>177</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -9907,10 +9903,10 @@
         <v>177</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -10174,10 +10170,10 @@
         <v>170</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -10441,10 +10437,10 @@
         <v>170</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -10708,10 +10704,10 @@
         <v>170</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -10975,10 +10971,10 @@
         <v>173</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -11242,10 +11238,10 @@
         <v>177</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -11509,10 +11505,10 @@
         <v>177</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -11793,7 +11789,7 @@
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="101" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B1" s="102" t="s">
         <v>1</v>
@@ -12066,10 +12062,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="110" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F2" s="110" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G2" s="109"/>
       <c r="H2" s="109"/>
@@ -12090,13 +12086,13 @@
         <v>36</v>
       </c>
       <c r="D3" s="114" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E3" s="114" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F3" s="113" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G3" s="105"/>
       <c r="H3" s="105"/>
@@ -12118,10 +12114,10 @@
         <v>145</v>
       </c>
       <c r="E4" s="116" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F4" s="116" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G4" s="105"/>
       <c r="H4" s="105"/>
@@ -12143,10 +12139,10 @@
         <v>145</v>
       </c>
       <c r="E5" s="116" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F5" s="116" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G5" s="105"/>
       <c r="H5" s="105"/>
@@ -12168,10 +12164,10 @@
         <v>147</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F6" s="116" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G6" s="105"/>
       <c r="H6" s="105"/>
@@ -12193,10 +12189,10 @@
         <v>147</v>
       </c>
       <c r="E7" s="116" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F7" s="116" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G7" s="105"/>
       <c r="H7" s="105"/>
@@ -12218,10 +12214,10 @@
         <v>149</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F8" s="116" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G8" s="105"/>
       <c r="H8" s="105"/>
@@ -12243,10 +12239,10 @@
         <v>149</v>
       </c>
       <c r="E9" s="116" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F9" s="116" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G9" s="105"/>
       <c r="H9" s="105"/>
@@ -12268,10 +12264,10 @@
         <v>145</v>
       </c>
       <c r="E10" s="116" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F10" s="116" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G10" s="105"/>
       <c r="H10" s="105"/>
@@ -12293,10 +12289,10 @@
         <v>145</v>
       </c>
       <c r="E11" s="116" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F11" s="116" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G11" s="105"/>
       <c r="H11" s="105"/>
@@ -12318,10 +12314,10 @@
         <v>147</v>
       </c>
       <c r="E12" s="116" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F12" s="116" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G12" s="105"/>
       <c r="H12" s="105"/>
@@ -12343,10 +12339,10 @@
         <v>147</v>
       </c>
       <c r="E13" s="116" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F13" s="116" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G13" s="105"/>
       <c r="H13" s="105"/>
@@ -12368,10 +12364,10 @@
         <v>149</v>
       </c>
       <c r="E14" s="116" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F14" s="116" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G14" s="105"/>
       <c r="H14" s="105"/>
@@ -12393,10 +12389,10 @@
         <v>149</v>
       </c>
       <c r="E15" s="116" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F15" s="116" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G15" s="105"/>
       <c r="H15" s="105"/>
@@ -16621,10 +16617,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16638,15 +16634,13 @@
     <col min="7" max="8" width="17.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="29.5" style="1" customWidth="1"/>
     <col min="10" max="11" width="20.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="22" style="1" customWidth="1"/>
-    <col min="16" max="16" width="45.33203125" style="1" customWidth="1"/>
-    <col min="17" max="19" width="8.83203125" style="1" customWidth="1"/>
-    <col min="20" max="1026" width="8.83203125" customWidth="1"/>
+    <col min="12" max="13" width="22" style="1" customWidth="1"/>
+    <col min="14" max="14" width="45.33203125" style="1" customWidth="1"/>
+    <col min="15" max="17" width="8.83203125" style="1" customWidth="1"/>
+    <col min="18" max="1024" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -16672,10 +16666,8 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-    </row>
-    <row r="2" spans="1:19" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:17" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="13" t="s">
@@ -16701,28 +16693,22 @@
         <v>185</v>
       </c>
       <c r="K2" s="121" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>186</v>
+        <v>116</v>
       </c>
       <c r="M2" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="N2" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="O2" s="13" t="s">
+      <c r="N2" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="P2" s="40" t="s">
-        <v>188</v>
-      </c>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-    </row>
-    <row r="3" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -16733,49 +16719,43 @@
         <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="K3" s="122" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="L3" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>199</v>
-      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>42736</v>
       </c>
@@ -16787,10 +16767,10 @@
         <v>173</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G4" s="4">
         <v>1</v>
@@ -16803,22 +16783,18 @@
         <v>1</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>202</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="N4" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="O4" s="4"/>
-      <c r="P4" s="3" t="s">
-        <v>172</v>
-      </c>
+      <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-    </row>
-    <row r="5" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>42736</v>
       </c>
@@ -16830,10 +16806,10 @@
         <v>173</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
@@ -16846,20 +16822,16 @@
         <v>2</v>
       </c>
       <c r="K5" s="120" t="s">
-        <v>270</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-    </row>
-    <row r="6" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>42736</v>
       </c>
@@ -16871,10 +16843,10 @@
         <v>173</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G6" s="4">
         <v>2</v>
@@ -16887,22 +16859,18 @@
         <v>1</v>
       </c>
       <c r="K6" s="120" t="s">
-        <v>270</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="N6" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="O6" s="4"/>
-      <c r="P6" s="3" t="s">
-        <v>172</v>
-      </c>
+      <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-    </row>
-    <row r="7" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>42736</v>
       </c>
@@ -16914,10 +16882,10 @@
         <v>173</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -16926,22 +16894,18 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="120" t="s">
-        <v>270</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="N7" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="O7" s="4"/>
-      <c r="P7" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-    </row>
-    <row r="8" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>42736</v>
       </c>
@@ -16953,10 +16917,10 @@
         <v>173</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -16965,22 +16929,18 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="120" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="O8" s="3"/>
+        <v>205</v>
+      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-    </row>
-    <row r="9" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>42736</v>
       </c>
@@ -16992,10 +16952,10 @@
         <v>170</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
@@ -17008,20 +16968,16 @@
         <v>1</v>
       </c>
       <c r="K9" s="120" t="s">
-        <v>270</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="N9" s="3"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="3"/>
+      <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-    </row>
-    <row r="10" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>42736</v>
       </c>
@@ -17033,10 +16989,10 @@
         <v>170</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G10" s="4">
         <v>2</v>
@@ -17051,22 +17007,18 @@
         <v>1</v>
       </c>
       <c r="K10" s="120" t="s">
-        <v>197</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3" t="s">
         <v>176</v>
       </c>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-    </row>
-    <row r="11" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>42736</v>
       </c>
@@ -17078,10 +17030,10 @@
         <v>170</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G11" s="4">
         <v>2</v>
@@ -17096,24 +17048,20 @@
         <v>2</v>
       </c>
       <c r="K11" s="120" t="s">
-        <v>270</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="P11" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>172</v>
       </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-    </row>
-    <row r="12" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>42736</v>
       </c>
@@ -17125,10 +17073,10 @@
         <v>170</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G12" s="4">
         <v>1</v>
@@ -17141,22 +17089,18 @@
         <v>1</v>
       </c>
       <c r="K12" s="120" t="s">
-        <v>270</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="N12" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="O12" s="4"/>
-      <c r="P12" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-    </row>
-    <row r="13" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="4"/>
@@ -17174,10 +17118,8 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-    </row>
-    <row r="14" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="4"/>
@@ -17195,10 +17137,8 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-    </row>
-    <row r="15" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="4"/>
@@ -17216,10 +17156,8 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-    </row>
-    <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="4"/>
@@ -17237,10 +17175,8 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-    </row>
-    <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="8"/>
@@ -17258,8 +17194,6 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -17291,7 +17225,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>1</v>
@@ -17312,10 +17246,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F2" s="49" t="s">
         <v>156</v>
@@ -17332,7 +17266,7 @@
         <v>36</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="50" t="s">
         <v>37</v>

</xml_diff>